<commit_message>
started to work on the new way we view items, either through comparison or expanded details.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Armour/body.xlsx
+++ b/resources/data-imports/Armour/body.xlsx
@@ -797,11 +797,11 @@
   </sheetPr>
   <dimension ref="A1:BR60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BN60" activeCellId="0" sqref="BN60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL61" activeCellId="0" sqref="AL61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.23"/>
@@ -7769,22 +7769,22 @@
         <v>73</v>
       </c>
       <c r="AH60" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI60" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ60" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK60" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL60" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN60" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR60" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Created a form wizard, started to use it.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Armour/body.xlsx
+++ b/resources/data-imports/Armour/body.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="190">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -584,6 +584,12 @@
   </si>
   <si>
     <t xml:space="preserve">Etched with ancient runes, this jerkin hums with latent magical power.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shattered Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A shattered crystal was turned into a a magical piece of armour</t>
   </si>
 </sst>
 </file>
@@ -797,8 +803,8 @@
   </sheetPr>
   <dimension ref="A1:BR60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL61" activeCellId="0" sqref="AL61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF60" activeCellId="0" sqref="AF60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7726,6 +7732,21 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="J60" s="2" t="n">
         <v>1999954324.58731</v>
       </c>

</xml_diff>